<commit_message>
Add actions and action fieldd descriptions for kommunen
</commit_message>
<xml_diff>
--- a/data/muenster/actions_raw.xlsx
+++ b/data/muenster/actions_raw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\workspace\klimawatch-django\data\muenster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1382CBF6-8F20-44CE-A0B0-7657B7CE01B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BC192B-B110-40A5-8B64-17792F65548B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CF4B38D8-16BC-4266-8C61-59A682587AC8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="155">
   <si>
     <t>Field</t>
   </si>
@@ -271,18 +271,568 @@
   <si>
     <t>Die Aufgabe dieser Stelle besteht einerseits darin, die Verwaltungsleitung undderen Ämter in allen landwirtschaftlichen Sachfragen zu beraten und andererseits als Ansprechpartner für die Münsteraner Landwirte zu fungieren, um ei-nen guten Austausch zwischen Stadtverwaltung und Landwirten zu gewährleisten. Diese Aufgabe kommt auch in vielen klimaschutzrelevanten Projekten zumTragen.</t>
   </si>
+  <si>
+    <t>Energetische und klimagerechte Quartierssanierung – Klimaschutz und Klima- anpassung im Quartier: zentrales Vorhaben zur Erhöhung der allgemeinen Sa- nierungsrate – Zukunftsfähige, nutzungsflexible Stadtquartiere fördern – Klima- schutz, Wohnangebote, Energieversorgung, Mobilität und Nahversorgung und weitere Themen in Münster integriert betrachten.</t>
+  </si>
+  <si>
+    <r>
+      <t>Der Rat der Stadt Münster hat am 26. August 2020 die überarbeiteten Gebäu- deleitlinien mit einem Änderungsantrag für Münster beschlossen. Der Energie- verbrauch der städtischen Gebäude soll bis zum Jahr 2030 um 50 % sowie die CO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>-Emissionen um 70 % reduziert werden. Sowohl für Neubau- als auch für Umbau- und Sanierungsmaßnahmen gibt es verbindliche Qualitätskriterien und eine Richtschnur für alle am Bauprozess städtischer Gebäude Beteiligten. Die Gebäudeleitlinien gelten dabei für alle Gebäude der Stadt Münster. Die städti- schen Tochterunternehmen wurden laut Beschluss auch aufgefordert, die Ge-
+bäudeleitlinien zu beschließen und anzuwenden.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Umstellung auf CO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>-freie Wärme- und Warmwasserversorgung des Gebäude- bestands  und  Verbrauchsreduktion:  Dämmung,  Teil-  und  Vollsanierung,  Be- triebsoptimierung</t>
+    </r>
+  </si>
+  <si>
+    <t>Thermografiebefliegung MS</t>
+  </si>
+  <si>
+    <t>Das Projekt setzt sich aus drei Phasen zusammen:
+1.   Thermografiebefliegung: Aufnahme der Wärmebilder von Münsters Dachlandschaft und Datenauswertung
+2.   Anschreiben der Hauseigentümer*innen sowie Beratungsangebot zur energetischen Sanierung 3.   Fortlaufende kostenfreie Energieberatung, Zustellung und Interpreta- tionsunterstützung bei der Auswertung der Thermografieaufnahmen</t>
+  </si>
+  <si>
+    <r>
+      <t>Die Stadt Münster fördert mit dem Förderprogramm vielfältige Maßnahmen zur energetischen Optimierung von Wohngebäuden im Stadtgebiet. Von der Ge- bäudedämmung  und  dem  Heizungsaustausch  über  Dachbegrünung  bis  zu ökologischen Dämmstoffen gibt es viele Möglichkeiten, einen wichtigen Beitrag
+zur Reduzierung der CO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>-Emissionen in Münster zu leisten.</t>
+    </r>
+  </si>
+  <si>
+    <t>PV-Anlagen auf städtischen Gebäuden</t>
+  </si>
+  <si>
+    <t>Bei allen zukünftigen Neu- und Erweiterungsbauten werden Dachflächen voll- flächig mit PV-Anlagen ausgestattet, Ratsvorlage wird erstellt und kommt vor der Sommerpause 2024 in die Beratungskette.</t>
+  </si>
+  <si>
+    <t>Leitfaden klimagerechte Bauleitplanung</t>
+  </si>
+  <si>
+    <t>Der Planungsleitfaden listet die Belange von Klimaschutz und Klimaanpassung auf, die in den jeweiligen Planungsphasen berücksichtigt werden müssen.</t>
+  </si>
+  <si>
+    <t>Münsters    „Standard    für    klimagerechtes Bauen“   in   „Grundstückskaufverträgen   und städtebaulichen Verträgen“</t>
+  </si>
+  <si>
+    <r>
+      <t>Durch  die  Kombination  aus  dem  Standard  „KfW-Effizienzhaus-/gebäude  40“ und  dem  Solarstandard  wird  der  CO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>-Ausstoß  beim  Betrieb  von  Neubauten deutlich gesenkt und je nach Gebäude bilanziell auch ein Plus-Energie-Stan-
+dard erreicht, mit dem das Gebäude über das Jahr mehr Energie erzeugt, als es verbraucht.</t>
+    </r>
+  </si>
+  <si>
+    <t>Energetische und klimagerechte Quartierssanierung</t>
+  </si>
+  <si>
+    <t>Gebäudeleitlinien bzw. energetischer Standard für Neubauten</t>
+  </si>
+  <si>
+    <t>Gebäudeleitlinien/Standards Neubauten</t>
+  </si>
+  <si>
+    <t>Quartierssanierung</t>
+  </si>
+  <si>
+    <t>Sanierungsstrategie Wohn- und  Stadtbau GmbH</t>
+  </si>
+  <si>
+    <t>Förderprogramm  klimafreundliche  Wohngebäude</t>
+  </si>
+  <si>
+    <t>Standard    für    klimagerechtes Bauen</t>
+  </si>
+  <si>
+    <t>Ausbau öffentlicher Ladeinfrastruktur</t>
+  </si>
+  <si>
+    <t>Die  öffentliche  Ladeinfrastruktur  soll  fortlaufend  weiterentwickelt  und  ausge- baut werden, sodass zukünftig ein flächendeckendes Angebot an Lademög-
+lichkeiten bereitgestellt werden kann und der Umstieg auf E-Fahrzeuge attrak- tiver wird.</t>
+  </si>
+  <si>
+    <t>Erweiterung E-Carsharing Angebot</t>
+  </si>
+  <si>
+    <t>Um den Umweltverbund zu stärken, den stadtweiten Kfz-Bestand zu reduzie- ren und den Zugang zum stadtweiten Carsharing-Angebot (auch E-Carsharing) zu verbessern, werden hierfür Flächen im Verkehrsraum bereitgestellt und po- tenziellen Anbietern im Ausschreibungsverfahren zur Verfügung gestellt.</t>
+  </si>
+  <si>
+    <t>Ausbau Mobilstationen</t>
+  </si>
+  <si>
+    <t>Durch den Ausbau von Mobilstationen soll die Vernetzung der Verkehrsträger – insbesondere die des Umweltverbundes – verbessert werden.
+Nach der Festlegung von Qualitätsstandards soll, nach entsprechendem politi- schem Beschluss über das Standortkonzept, ab 2024 die sukzessive Umset- zung erfolgen.</t>
+  </si>
+  <si>
+    <t>Parkraumkonzept</t>
+  </si>
+  <si>
+    <t>Es wird ein maßnahmenorientiertes Konzept zur Neuordnung und Anpassung des Parkraumangebots in der Innenstadt entwickelt. Die Ziele dabei sind, das sichtbare  Parken im  öffentlichen Raum  zu reduzieren und damit die Aufent- haltsqualität und Barrierefreiheit zu erhöhen. Hierbei sollen die Bewohnerpark-
+zonen ausgeweitet, ein Parkraumanagement eingeführt und das „faire Parken“ umgesetzt werden.</t>
+  </si>
+  <si>
+    <t>Fahrradnetz 2.0</t>
+  </si>
+  <si>
+    <r>
+      <t>Unter der Überschrift „Fahrradnetz 2.0“ wird eine Hierarchisierung und insge- samte Verbesserung des städtischen Radverkehrsnetzes angestrebt – mit dem Ziel, den Radverkehrsanteil am Umweltverbund weiter zu steigern und damit verkehrsbedingte CO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>-Emissionen zu reduzieren. Hierfür wurden im Rahmen
+der Konzepterstellung  verschiedene  Handlungsempfehlungen entwickelt, die Anfang 2024 in die politische Beratung eingebracht wurden.</t>
+    </r>
+  </si>
+  <si>
+    <t>Definition  eines  Rahmens  für  Dienstreisen,  der  Nachhaltigkeits-  und  Klima-
+schutzaspekte verbindlich einbezieht.</t>
+  </si>
+  <si>
+    <t>Um die Mitarbeitenden bei der Nutzung des Umweltverbunds für den Arbeits- weg zu unterstützen/zu supporten/zu fördern oder Anreize/Incentives zum Um- stieg vom MIV auf den Umweltverbund zu geben, befinden sich verschiedene Projekte in Planung oder sind bereits umgesetzt.</t>
+  </si>
+  <si>
+    <t>Reduzierung &amp; Elektrifizierung Fuhrpark</t>
+  </si>
+  <si>
+    <t>Der städtische Fuhrpark soll fortlaufend auf E-Mobilität umgestellt werden. Dies geschieht bereits bei vielen Ersatzbeschaffungen. Außerdem wird der Umfang
+des städtischen Fuhrparks kritisch analysiert, um Überkapazitäten abzubauen. Zur Beschleunigung und Systematisierung des Prozesses werden darüber hin- aus u. a. die folgenden Instrumente, Projekte und Begleitprozesse initiiert:
+     Sondierung Fahrzeugbestand
+     Weitere Verlagerung auf Carsharing
+     Einführung Fuhrparkmanagement (perspektivisch)
+     Dienstwagen-Pooling</t>
+  </si>
+  <si>
+    <t>S-Bahn-Münsterland</t>
+  </si>
+  <si>
+    <t>Der Schienenpersonennahverkehr soll in den nächsten Jahren massiv gestärkt und damit eine deutliche Verlagerung des Pendlerverkehrs vom motorisierten Individualverkehr  auf  den  Umweltverbund  insgesamt  erreicht  werden.  Dazu sollen neben zusätzlichen Zugfahrten auf den vorhandenen Strecken auch still- gelegte Bahntrassen reaktiviert und neue Haltepunkte gebaut werden.</t>
+  </si>
+  <si>
+    <t>Neukonzeption des bestehenden ÖPNV-An- gebotes</t>
+  </si>
+  <si>
+    <t>Das bestehende ÖPNV-Angebot wird fortan weiterentwickelt und -konzeptio- niert, mit dem Ziel, den Umweltverbund zu stärken und dadurch die verkehrs- bedingten Emissionen zu reduzieren. Ein zentraler Baustein dabei ist die Auf-
+stellung des Nahverkehrsplans.</t>
+  </si>
+  <si>
+    <t>Geschäftsanweisung „Dienstreisen und- gänge im Umweltverbund“</t>
+  </si>
+  <si>
+    <t>Geschäftsanweisung Dienstreisen</t>
+  </si>
+  <si>
+    <t>Ausbau von Mitarbeitendenmobilitäts-Angeboten</t>
+  </si>
+  <si>
+    <t>Neukonzeption des ÖPNV-Angebotes</t>
+  </si>
+  <si>
+    <t>Nachhaltige Geldanlagen</t>
+  </si>
+  <si>
+    <t>Die Stadt Münster legt Gelder insbesondere zur Reduzierung künftiger Versor- gungslasten für die  Pensionszahlungen an Beamt*innen in  zwei städtischen Spezialfonds an. Beim Versorgungs- und Sanierungsfonds (VUS-Fonds) ist die Stadt  Münster  alleinige  Anlegerin,  der  Westfälische-Versorgungs-Rücklage- Fonds (WVR-Fonds) ist ein Zusammenschluss von neun Kommunen. Seit dem Jahr 2016 erfolgt die Kapitalanlage nach nachhaltigen Kriterien. Die
+vom Fondsmanagement erworbenen Aktien und Unternehmensanleihen müs- sen  bestimmten  nachhaltigen  Kriterien  genügen.  Einige  Branchen  sind  voll- ständig  ausgeschlossen  (Fracking/Militärwaffen/Atomenergie/klimaschädliche Energie),  alle  anderen  Branchen  müssen  ein  bestimmtes  Nachhaltigkeitsni- veau  erreichen.  Bei  Unternehmensanleihen  muss  es  sich  um  sogenannte
+‚Green  Bonds‘  handeln.  Bestimmungen  zur  Nachhaltigkeit  der  Geldanlagen sind in der Anlagerichtlinie der Stadt Münster festgehalten.
+Darüber hinaus hat die Stadt Münster insbesondere in ihrem allein gehaltenen Fonds das ESG Reporting deutlich ausgebaut. Der ESG-Bericht und der CO2- Bericht sind mittlerweile fester Bestandteil der halbjährlichen Sitzung des Anla- geausschusses. Die Maßnahmen haben den CO2-Fußabdruck und das ESG- Rating  der  gehaltenen  Wertpapiere  und  damit  der  städtischen  Geldanlagen deutlich verbessert.
+Die Anlagenrichtlinie wurde nun weiterentwickelt und um Nachhaltigkeitskrite- rien erweitert. Erstmalig werden auch Investitions- bzw. Ausschlusskriterien für den Erwerb von Staatsanleihen definiert. Darüber hinaus müssen für Investiti- onen in Unternehmen/Staaten zukünftig bestimmte Einstufungen im ESG-Ra- ting erfüllt werden.</t>
+  </si>
+  <si>
+    <t>Stärkung von Nachhaltigkeitsberichterstattungen im Stadtkonzern.
+Die bestehenden Berichterstattungen im Stadtkonzern sind heterogen, da teil- weise Pflichten bestehen oder sich abzeichnen (EU-Richtlinie CSRD (Corpo- rate Sustainability Reporting Directive)) und teilweise andere Berichtsformate, wie die gemeinwohlorientierte Bilanz, in Nutzung sind.
+Die Nachhaltigkeitsberichterstattung der städtischen Beteiligungsgesellschaf-
+ten soll gestärkt werden. Hierzu wird es Empfehlungen im Rahmen des Public- Corporate-Governance-Kodex geben.</t>
+  </si>
+  <si>
+    <t>Einrichtung eines Bauinvestitionscontrollings</t>
+  </si>
+  <si>
+    <t>Der Antrag A-R/0053/2022 von Bündnis 90/Die Grünen, SPD und Volt an den Rat der Stadt Münster hat zum Inhalt, das „Controlling bezüglich Kosten für Bau und  Anmietung  zu  verbessern“.  Hierzu  fordert  die  Politik,  ein  unabhängiges Bauinvestitionscontrolling  aufzubauen und  zu etablieren. Dies soll insbeson- dere dazu dienen, die Investitionskosten im Blick zu haben und zu beurteilen,
+welche  Kostensteigerungen  tatsächlich  notwendig  sind.  Außerdem  soll  das Controlling einen kritischen Blick auf die Bedarfe der einzelnen Ämter werfen und prüfen, inwiefern diese tatsächlich notwendig sind. Politik, Immobilienma-
+nagement und die Bedarfsämter können dies aktuell nicht unabhängig prüfen.</t>
+  </si>
+  <si>
+    <t>Entwicklung eines Klimahaushaltes</t>
+  </si>
+  <si>
+    <t>Das Steuerungselement Finanzen soll mit Aussagen zu Klimawirkungen ver- bunden werden. Das Instrument Klimahaushalt soll dabei eine Hilfe sein, um zu verstehen, welche Klimaauswirkungen Finanzentscheidungen haben. Da es in Deutschland bisher keine Kommune mit einem echten Klimahaushalt gibt,
+bedarf es einer Konzeption, die als Prozess zu verstehen ist. Erste Ideen wur- den hierzu entwickelt und getestet.</t>
+  </si>
+  <si>
+    <t>Green Bonds/Grüner Schuldschein</t>
+  </si>
+  <si>
+    <t>Im September 2021 hat der Rat der Stadt Münster mit der Vorlage V/0666/2021 die  Verwaltung  beauftragt,  die  nachhaltige  Kapitalbeschaffung  über  einen Green Bond zu initiieren. Die Platzierung des Schuldscheins am Markt erfolgte im September 2022. Aufgrund des großen Interesses an dem Grünen Schuld- schein konnte das ursprüngliche Volumen von 100 auf 140 Mio. Euro erhöht und zugeteilt werden. Erfreulich war, dass alle Laufzeiten von 7 bis 20 Jahren auf Interesse der Investierenden gestoßen sind und bedient werden konnten. Insgesamt haben 16 Investierende den Schuldschein gezeichnet. Im Septem- ber 2023 wurde der 1. Allokations- und Wirkungsbericht zum Green Bond vor- gelegt. In dem Bericht wird über die Mittelverwendung (Allokationsbericht) und die  Nachhaltigkeitswirkung  der  finanzierten  Investitionen  beziehungsweise Projekte (Wirkungsbericht) Auskunft gegeben.
+Für das Jahr 2024 ist die Auflegung eines weiteren Green Bonds über 120 Mil- lionen Euro geplant.</t>
+  </si>
+  <si>
+    <t>Nachhaltigkeitsberichterstattung im Stadtkonzern</t>
+  </si>
+  <si>
+    <t>Bildung  für  nachhaltige  Entwicklung  fest  in schulischen und außerschulischen Bildungs-
+einrichtungen etablieren</t>
+  </si>
+  <si>
+    <t>Bildung für nachhaltige Entwicklung (BNE) bis 2030 fest in Bildungseinrichtun- gen zu etablieren, ist ein vom Rat der Stadt Münster beschlossenes Ziel der Stadt Münster. Schwerpunkte für das Jahr 2024 u. a. mit Schwerpunkt Klima und Ernährung sind:
+- Weiterentwicklung des Münsteraner BNE-Netzwerkes (2 – 3 Vernetzungstref- fen; nächstes gemeinsames Bildungsprogramm für das Schuljahr 2023/2024 entwickeln, nächste gemeinsame BNE-Fachtagung im Herbst 2024; Entwick- lung eines Newsletters)
+- Unterstützung von „Schule der Zukunft“: Anwerben weiterer Schulen; Durch- führung von 1 – 2 ganztägigen BNE-Modulen (für Lehrer*innen oder weitere Pädagog*innen)  und  1  –  2  Schüler*innenakademien  (schulübergreifend  für Schüler*innen);  Aufbau  des  Münsteraner  Schulnetzwerkes  „Schule  der  Zu- kunft“
+- Umsetzung des Grundschulprojekts „YooLe – raus aus Schule“ mit derzeit 7 beteiligten Grundschulen und Weiterentwicklung und Ausdehnung des Ange- bots für das Schuljahr 2024/2025
+- Umsetzung des vielfältigen Bildungsprogramms in Kooperation mit Haus Heit- horn
+- Weiterführung des „Zukunftsdiploms“ als Kooperationsprojekt des BNE-Regi- onalzentrums mit der vhs Münster
+- Weiterentwicklung des  Schulgartennetzwerkes mit beteiligten Schulen (ge- meinsame Obsternte auf der Streuobstwiese Haus Kump; Apfelversaftungsak- tion mit beteiligten Grundschulen; Austauschtreffen)
+- Aktionstage zum Aufstellen und Erstbepflanzen von 12 neuen Hochbeeten an unterschiedlichen Schulen  (Kooperationsprojekt mit dem  Adolph-Kolping-Be- rufskolleg)
+- Einführung einer regelmäßigen „BNE-Sprechstunde“ im Haus der Nachhaltig- keit
+- Vergabe und Beratung zum städtischen Förderprogramm „Urbane Bürgergär- ten“</t>
+  </si>
+  <si>
+    <t>Umstellung Kantinenessen</t>
+  </si>
+  <si>
+    <t>Ziele:
+Mit der Vorlage V/0669/2019 hat der Rat der Stadt Münster folgendes Ziel be- schlossen: „Die Verpflegung in den städtischen Kantinen erfolgt zunehmend
+aus biologischem Anbau, fair, regional und saisonal. Feste Bestandteile des Speiseplans sind vegetarische und vegane Angebote.“ Mit der Vorlage V/0731/2021 wurde das Maßnahmenprogramm Klimaneutrale Stadtverwaltung 2030 beschlossen. Darin heißt es konkret: „Städtische Veran- staltungen, die Mittagsverpflegung in den Kantinen und die Ratsarbeit erfolgen nachhaltig und klimaneutral.“
+Bis 2022:
+Die Verpflegung in den städtischen Kantinen ist zu 20 % auf faire, saisonale und regionale Bio-Lebensmittel umgestellt. 33 % der Gerichte sind vegetarisch. Bis 2030:
+- Der Lebensmittelbedarf wird, sofern verfügbar, vollständig aus umweltscho- nenden, saisonal produzierten Bio-Lebensmitteln der Region gedeckt. Gilt auch für kommunale Einrichtungen und Betriebe (im Rahmen der zur Verfügung ste- henden Budgets).
+Für  die  Zielerreichung  werden  verschiedene  Teilprojekte  erforderlich  sein. Zentraler Ansatz ist derzeit die Bewerbung der städtischen Kantine für das Kan- tinenprogramm NRW der Verbraucherzentrale NRW: Die Verbraucherzentrale NRW bietet fachliche Beratung, um Einrichtungen in öffentlicher Trägerschaft bei der Optimierung des Verpflegungsangebotes zu begleiten. Kantinen wer- den dabei unterstützt, das Verpflegungsangebot attraktiv und gesundheitsför- dernd auszurichten, Lebensmittelabfälle  zu reduzieren und das Bewusstsein für mehr Wertschätzung von Lebensmitteln zu stärken. Zudem erhalten sie Im-
+pulse für die Beschaffung von regional erzeugten Lebensmitteln. Ob die städti- sche Kantine für das Programm ausgewählt wird, ist noch offen.</t>
+  </si>
+  <si>
+    <t>KlimaTraining skalieren</t>
+  </si>
+  <si>
+    <t>Das KlimaTraining der Stadt Münster ist ein langfristiges Projekt. Es soll einen
+„Schneeballeffekt“ zur Aktivierung und Qualifizierung der Münsteraner Bevöl- kerung hin zu klimafreundlichen Verhaltensweisen unterstützen und damit die Transformation der Stadtgesellschaft bis 2030 vorantreiben.
+Das KlimaTraining findet aktuell zweimal jährlich in Kleingruppen mit circa fünf Teilnehmenden (Trainees) statt. Die jeweiligen Gruppen werden von ehrenamt- lichen KlimaTrainer*innen moderiert. Im KlimaTraining erarbeiten die Teilneh- menden  (Trainees)  individuelle  Klimaschutzmaßnahmen  und  erhalten  Gele- genheit, klimafreundliche Angebote auszuprobieren und zu testen. Hierzu wird
+von Münsteraner Unternehmen und Organisationen ein Portfolio von circa 15 Angeboten  in  den  Bereichen Wohnen und  Energie,  Mobilität sowie  Konsum und Ernährung dauerhaft bereitgestellt. Die Aktualität der Angebote wird tur- nusmäßig geprüft und es werden eventuelle Anpassungen im Angebotsportfo- lio durchgeführt.
+Der Ansatz des KlimaTrainings soll über eine zielgruppenspezifischere Ausge- staltung skaliert werden. KlimaTraining macht Schule: KlimaTraining wird als Projektkurs  an  der  Mathilde-Anneke-Gesamtschule  etabliert,  teilnehmende Schüler*innen werden zu KlimaTrainer*innen ausgebildet und begleiten Schü- ler*innen aus der Unterstufe oder in den Grundschulen.</t>
+  </si>
+  <si>
+    <t>Sachstand: Die Anforderungen an die Qualität der Mittagsverpflegung in Schu- len steigen (Ratsanträge 2022/Bürgeranregung § 24 GO). Die Verwaltung hat deshalb bei den jüngsten Ausschreibungen den geforderten Anteil des Einsat- zes biozertifizierter Lebensmittel von 20 % auf 30 % erhöht. Gleichzeitig sinkt mit dem  eingeleiteten Wechsel der OGS-Trägerschaft von  der Stadt  zu den freien Trägern der Einfluss der Stadt auf die Ausgestaltung der Verpflegung an den  Grundschulen.  Im  Rahmen  der  Überarbeitung  der  OGS-Qualitätsstan- dards soll der Aspekt klimafreundliche Ernährung  weiterverfolgt werden. Für die Ausschreibungen der Mittagsverpflegung an den weiterführenden Schulen können klimafreundliche Aspekte im Rahmen der Leistungsverzeichnisse be- rücksichtigt werden, soweit dies im Vergaberecht zulässig ist. Die Leistungs- verzeichnisse sehen den anteiligen Einsatz von biologischen, saisonalen und
+fair produzierten Lebensmitteln vor.</t>
+  </si>
+  <si>
+    <t>Bildungsarbeit Klimaschutz</t>
+  </si>
+  <si>
+    <r>
+      <t>Ziel: Münsteraner*innen aller Alters- und Lebensphasen zu klimaschonenden Lebensstilen ermutigen und so die Verankerung in der Stadtgesellschaft voran- treiben. Beispiele klimaschonenden Verhaltens sollen zielgruppengerecht auf- bereitet, Verhaltensänderungen angestoßen werden, um verhaltensbezogene CO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>-Reduktionspotenziale zu nutzen. Die Angebote der vhs sowie der Stadt- bücherei in den Bereichen Umweltbildung, Klimaschutz, Nachhaltigkeit stoßen
+bereits auf großes Interesse und sollen verstetigt/ausgebaut werden.</t>
+    </r>
+  </si>
+  <si>
+    <t>Biostadt    Münster    und    Ökomodellregion Münsterland</t>
+  </si>
+  <si>
+    <t>Vom Rat der Stadt Münster wurden mit Bezug auf das Jahr 2030 folgende Ziele beschlossen:
+- Regionale Wertschöpfungsprozesse aktiv zu unterstützen,
+- Verpflegung in städtischen Kantinen, Schulen und Kitas zunehmend bio, fair, regional, vegetarisch und vegan ausrichten, Lebensmittelbedarf (sofern verfüg- bar)  zu 100 % aus umweltschonenden, saisonal produzierten  Lebensmitteln der Region decken und
+- die Anteile der ökologischen Landwirtschaft auf mindestens 5 % bis 2030 und ebenfalls  die  Anteile  einer  nachhaltigeren  konventionellen  Landwirtschaft  zu steigern.</t>
+  </si>
+  <si>
+    <t>„TrinkWasser“-Kampagne</t>
+  </si>
+  <si>
+    <r>
+      <t>Ziele:
+-     Bereitstellung von Trinkwasser im öffentlichen Raum
+-     Klimaschutz (CO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>-Reduktion)/Hitzevorsorge/Gesundheitsförderung
+-     Bildung und Information
+Teilprojekte:
+-     Bau von Trinkbrunnen, damit Trinkwasser an öffentlichen Orten bereitge- stellt wird. Hierbei soll, soweit möglich, an die bestehende Infrastruktur (z. B. öffentliche WC-Anlagen, historische Brunnen) angedockt werden.
+-     Anwerben weiterer Refill-Standorte (https://refill-deutschland.de/muens- ter/) im gesamten Stadtgebiet, insbesondere in den äußeren Stadtteilen, und Steigerung des Bekanntheitsgrades durch öffentlichkeitswirksame Maßnahmen.
+Informationskampagne „TrinkWasser“ zu den Vorteilen von Leitungswasser (zu Hause frisch  aus dem  Hahn  und  jederzeit  verfügbar, ständige Qualitätskon- trolle, gesund,  weil keine  Kalorien und viele Mineralstoffe, preiswert, ca. ein
+Cent für zwei Liter, besonders nachhaltig, weil abfallfrei und kein CO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>für Trans- port und Verpackung)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Bildung  für  nachhaltige  Entwicklung </t>
+  </si>
+  <si>
+    <t>Klimafreundliche Mittagsverpflegung in Schulen</t>
+  </si>
+  <si>
+    <t>Biostadt  Münster    und    Ökomodellregion Münsterland</t>
+  </si>
+  <si>
+    <t>Ökoprofit</t>
+  </si>
+  <si>
+    <t>138 Unternehmen/Institutionen aus Münster profitieren bereits von Einsparun-
+gen,  die  sie  durch  ihre  Teilnahme  am  Beratungsprojekt  Ökoprofit®  (Amt für Grünflächen, Umwelt und Nachhaltigkeit) erzielen konnten: Ein Jahr lang stel- len Unternehmen und Nachhaltigkeitsberater*innen alle Abläufe eines Betrie- bes auf den Prüfstand: In Workshops und bei Vor-Ort-Beratungen werden kon- krete     Maßnahmen     entwickelt     und     umgesetzt,     Auszeichnung     aller Teilnehmenden als „Ökoprofit-Unternehmen“.
+Bei den bisher 13 Durchgängen des Projektes konnten insgesamt 20.108 Ton-
+nen CO2  eingespart werden.</t>
+  </si>
+  <si>
+    <t>Wasserstoff</t>
+  </si>
+  <si>
+    <t>- Wasserstoff-Koordinator  bei der  Technologieförderung  Münster GmbH seit April 2023: Wasserstoffstrategie für den Wirtschaftsstandort Münster
+-  H2inBatCellProd  (Technologieförderung,  Fraunhofer  FFB,  Westfalen  AG, Stadtwerke, Stadtnetze): Einsatz von Grünem Wasserstoff als Energieträger für Trocknungsstrecken und Trockenräume in der Batteriezellproduktion</t>
+  </si>
+  <si>
+    <t>Allianz für Klimaschutz</t>
+  </si>
+  <si>
+    <r>
+      <t>Zusammenschluss von rund 100 Münsteraner Unternehmen, die sich den städ- tischen Klimaschutzzielen verschrieben haben und hierfür jedes Jahr eine CO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>- Grobbilanz und eine Klimaschutzmaßnahme erarbeiten. Im Gegenzug erhalten sie dafür von der Stadt eine Begleitung und Unterstützung: vier- bis fünfjährli- che Netzwerktreffen, vier Newsletter pro Jahr, verschiedene Beratungsange-
+bote (5 bis 10 Beratungen pro Jahr), Öffentlichkeitsarbeit. Für die Unternehmen ist die Mitgliedschaft kostenfrei.</t>
+    </r>
+  </si>
+  <si>
+    <t>Standortentwicklungsstrategie 2030+</t>
+  </si>
+  <si>
+    <t>Verankerung des Ziels der Klimaneutralität als strategische Leitlinie in der Stan- dortentwicklungsstrategie 2030+, z. B. klimaneutrale Gewerbegebiete, Ausbau der Infrastrukturen für klimaneutrales Wirtschaften z. B. H2-Netze und Grüne Energie,  Stärkung  und  Weiterentwicklung  Münsters  als  Batterieforschungs-,
+Produktions-, Nutzungs- und Recyclingstandort, Entwicklung der GreenTech- Region Münsterland</t>
+  </si>
+  <si>
+    <t>Wirtschaftsförderung:  Informationsveranstal- tungen, Workshops, Podcast</t>
+  </si>
+  <si>
+    <t>Informationsveranstaltungen, Workshops, Podcast der Wirtschaftsförderung zu Nachhaltigkeit und Klimaschutz</t>
+  </si>
+  <si>
+    <t>Klimastadt-Vertrag</t>
+  </si>
+  <si>
+    <t>Im Klimastadt-Vertrag veröffentlichen Münsteraner*innen ihren Beitrag auf dem Weg zur Klimastadt, verpflichten sich dadurch und inspirieren und motivieren weitere  Unterstützer*innen.  Weil  es  uns  alle  braucht!  Beginnend  mit  dem Stadtforum im Juni 2023 können alle Münsteraner*innen – egal ob Unterneh-
+men, Bürger*in, Verein oder andere Einrichtung – Maßnahmen benennen, die sie selbst umsetzten und so als Beitrag zur Klimastadt zum Klimastadt-Vertrag beisteuern wollen. Jeder Beitrag auf dem Weg zur Klimaneutralität zählt. In ei-
+nem intensiven Dialog mit Wirtschaft und Hochschulen werden Beiträge zum Klimastadt-Vertrag erarbeitet.</t>
+  </si>
+  <si>
+    <t>Klimaneutrale Gewerbegebiete – im Bestand und in der Entwicklung</t>
+  </si>
+  <si>
+    <t>Kreislaufstadt</t>
+  </si>
+  <si>
+    <t>Deutsches Institut für Urbanistik, Deutscher Städtetag, 22 Kommunen (Wirt- schaftsförderung): Im Städteverbund wird ein Modellansatz bestehend aus den Komponenten Leitbild und Ziele, Strategie, Prozesse, Strukturen, Instrumente
+und Produkte für die Entwicklung von ganzheitlichen kommunalen Kreislauf- wirtschaftsstrategien erarbeitet.</t>
+  </si>
+  <si>
+    <t>Startberatung Energieeffizienz</t>
+  </si>
+  <si>
+    <t>Klimaschutz-Beratungsangebot für kleine und mittlere Unternehmen mit dem Schwerpunkt Energieeinsparung  und nachhaltiger,  effizienter  Energieeinsatz auf Basis erneuerbarer Energien
+Ziel: ganz konkrete Klimaschutzmaßnahmen in den Unternehmen auf den Weg
+bringen. Niedrigschwelliges Angebot: keine Anträge, Formulare, Kosten für das Unternehmen.</t>
+  </si>
+  <si>
+    <t>Wirtschaftsförderung</t>
+  </si>
+  <si>
+    <t>Klimaneutrale Gewerbegebiete</t>
+  </si>
+  <si>
+    <t>1. Bestandsgewerbegebiete klimaneutral umgestalten: Besetzung einer neuen Stelle  bei  der Wirtschaftsförderung  zum  1.  Januar  2024,  2024  Analyse  und Umsetzung erster Maßnahmen 2.  Neue  Gewerbegebiete:  u.  a.  Gewerbegebiet  Gelmer  –  nördlich  Heit- mannsweg    (Bebauungsplanverfahren    mit    dem    Ziel    „klimapositiv“    mit Ratsbeschluss   22.03.2023   eingeleitet),   Modellquartier   Busso-Peus-Straße (zweiphasiger städtebaulicher Wettbewerb: Ratsbeschluss 10.05.2023 – klima- positive   Entwicklung,   Preisgericht   15.02.2024),   Modellquartier   Steinfurter Straße    (Werkstattverfahren    abgeschlossen,    Ratsbeschluss    10.05.2023,
+Beschluss, Auslobung, Wettbewerb Mitte 2024: klimapositive Entwicklung) ...</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -293,7 +843,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -301,14 +851,60 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF5D8692"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF5D8692"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF5D8692"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF5D8692"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF5D8692"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF5D8692"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF5D8692"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -644,16 +1240,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79967D0A-D213-4CC7-8CC6-78949D60D9F9}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="106.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="141.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="255.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="115.28515625" bestFit="1" customWidth="1"/>
@@ -746,16 +1342,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
         <v>20</v>
@@ -766,13 +1362,13 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
         <v>20</v>
@@ -783,13 +1379,13 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
         <v>20</v>
@@ -800,13 +1396,13 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E9" t="s">
         <v>20</v>
@@ -817,219 +1413,882 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" t="s">
-        <v>35</v>
+        <v>37</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="E11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>45</v>
+        <v>18</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
       </c>
       <c r="E15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="51" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>46</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B24" t="s">
         <v>47</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C24" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="E24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>49</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B35" t="s">
         <v>50</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C35" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="E35" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E36" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="51" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E37" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="51" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E38" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E39" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="E40" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>52</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B41" t="s">
         <v>53</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C41" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="E41" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="140.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42" t="s">
+        <v>132</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E42" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="140.25" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E43" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="102" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E44" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E45" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E46" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="51" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E47" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E48" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>55</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B49" t="s">
         <v>56</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C49" t="s">
         <v>56</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D49" t="s">
         <v>57</v>
       </c>
-      <c r="E19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="E49" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E50" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>55</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E51" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E52" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E53" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E54" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="51" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E55" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="51" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="E56" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>55</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E57" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>55</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E58" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>58</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B59" t="s">
         <v>59</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C59" t="s">
         <v>59</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D59" t="s">
         <v>60</v>
       </c>
-      <c r="E20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="E59" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>58</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B60" t="s">
         <v>61</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C60" t="s">
         <v>62</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D60" t="s">
         <v>63</v>
       </c>
-      <c r="E21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="E60" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>64</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B61" t="s">
         <v>65</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C61" t="s">
         <v>66</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D61" t="s">
         <v>67</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E61" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>